<commit_message>
bug fix in convenios
</commit_message>
<xml_diff>
--- a/files/reporte-movilidad-entrada.xlsx
+++ b/files/reporte-movilidad-entrada.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Id</t>
   </si>
@@ -91,6 +91,48 @@
     <t>Autor</t>
   </si>
   <si>
+    <t>periodo5</t>
+  </si>
+  <si>
+    <t>Mexicali</t>
+  </si>
+  <si>
+    <t>FAC. DE CIENCIAS HUMANAS</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Doriga</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Doctorado</t>
+  </si>
+  <si>
+    <t>SAUZAL</t>
+  </si>
+  <si>
+    <t>MEXICO</t>
+  </si>
+  <si>
+    <t>BAJA CALIFORNIA</t>
+  </si>
+  <si>
+    <t>espanol</t>
+  </si>
+  <si>
+    <t>Estancia de Investigacion</t>
+  </si>
+  <si>
+    <t>judith</t>
+  </si>
+  <si>
     <t>2022-2</t>
   </si>
   <si>
@@ -112,61 +154,43 @@
     <t>Femenino</t>
   </si>
   <si>
-    <t>Doctorado</t>
-  </si>
-  <si>
-    <t>SAUZAL</t>
-  </si>
-  <si>
-    <t>MEXICO</t>
-  </si>
-  <si>
-    <t>BAJA CALIFORNIA</t>
-  </si>
-  <si>
     <t>ESPAÑOL</t>
   </si>
   <si>
     <t>Estancias Sabaticas</t>
   </si>
   <si>
-    <t>judith</t>
-  </si>
-  <si>
-    <t>periodo</t>
-  </si>
-  <si>
-    <t>destino</t>
-  </si>
-  <si>
-    <t>unidaddd</t>
-  </si>
-  <si>
-    <t>fernanada</t>
-  </si>
-  <si>
-    <t>alcala</t>
-  </si>
-  <si>
-    <t>perrez</t>
-  </si>
-  <si>
-    <t>Licenciatura</t>
-  </si>
-  <si>
-    <t>medicina</t>
-  </si>
-  <si>
-    <t>mexico</t>
-  </si>
-  <si>
-    <t>sonora</t>
-  </si>
-  <si>
-    <t>español</t>
-  </si>
-  <si>
-    <t>Estancia de Investigacion</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Ensenada</t>
+  </si>
+  <si>
+    <t>FACULTAD DE CIENCIAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juana </t>
+  </si>
+  <si>
+    <t>de Arco</t>
+  </si>
+  <si>
+    <t>salen</t>
+  </si>
+  <si>
+    <t>Maestria</t>
+  </si>
+  <si>
+    <t>Universidad de Oaxaca</t>
+  </si>
+  <si>
+    <t>Oaxaca</t>
+  </si>
+  <si>
+    <t>Docencia</t>
+  </si>
+  <si>
+    <t>jluna@uabc.edu.mx</t>
   </si>
 </sst>
 </file>
@@ -547,7 +571,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="26" width="10" customWidth="1"/>
@@ -635,28 +659,28 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>354321</v>
+        <v>65465</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
       </c>
       <c r="D2">
-        <v>324354</v>
+        <v>35435</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
       </c>
       <c r="F2">
-        <v>35435</v>
+        <v>65465</v>
       </c>
       <c r="G2" t="s">
         <v>28</v>
       </c>
       <c r="H2">
-        <v>54354</v>
+        <v>54654</v>
       </c>
       <c r="I2" t="s">
         <v>29</v>
@@ -668,7 +692,7 @@
         <v>31</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2" t="s">
         <v>32</v>
@@ -683,10 +707,10 @@
         <v>2</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S2" t="s">
         <v>34</v>
@@ -701,7 +725,7 @@
         <v>37</v>
       </c>
       <c r="W2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -715,28 +739,28 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>9999</v>
+        <v>354321</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
       </c>
       <c r="D3">
-        <v>62155</v>
+        <v>324354</v>
       </c>
       <c r="E3" t="s">
         <v>41</v>
       </c>
       <c r="F3">
-        <v>5435435</v>
+        <v>35435</v>
       </c>
       <c r="G3" t="s">
         <v>42</v>
       </c>
       <c r="H3">
-        <v>4524</v>
+        <v>54354</v>
       </c>
       <c r="I3" t="s">
         <v>43</v>
@@ -751,46 +775,126 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="P3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
       <c r="R3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" t="s">
+        <v>36</v>
+      </c>
+      <c r="V3" t="s">
         <v>47</v>
       </c>
-      <c r="T3" t="s">
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="s">
         <v>48</v>
-      </c>
-      <c r="U3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V3" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>51</v>
       </c>
       <c r="Z3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>2022</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>400</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" t="s">
+        <v>54</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U4" t="s">
+        <v>57</v>
+      </c>
+      <c r="V4" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>